<commit_message>
Accreditamento TESI SPA _ EMOWEB - Correzione testcase 191 - 376
Accreditamento TESI SPA _ EMOWEB - Correzione testcase 191 - 376
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250207\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250220\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B88180C-12E3-442A-8600-C8CB036CAEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FEA541-0885-4900-B9E5-3058F4A381AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1918,24 +1918,6 @@
     <t>subject_application_version: 3.3</t>
   </si>
   <si>
-    <t>2025-02-07T10:48:09.306Z</t>
-  </si>
-  <si>
-    <t>06e8c80cdf18e381</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.c73478e14f4885b6f353fc8bf6f9bfeb167441075f574f015b9bf71db10f47fd.a5ede5287d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>c88c8942000f9317</t>
-  </si>
-  <si>
-    <t>2025-02-07T10:38:01.988Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.fc02373146190d7bc0290b0ddc4cb97e647566b5425c3c19e45b48c7164186ba.f1554966d0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>EMOWEB è un software per il Trasfusionale, non per Laboratorio Analisi.</t>
   </si>
   <si>
@@ -2029,6 +2011,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.190208.6.11.b7e3599442e9321114b7a048d8b6ca9b583fb36ec4fab58754e98a9ff5f7abb7.99918db4c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-20T16:16:11.643Z</t>
+  </si>
+  <si>
+    <t>ec0fb70c78870364</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.7efbaea588^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>56e8705b885bb22f</t>
+  </si>
+  <si>
+    <t>2025-02-20T16:22:03.068Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.5f58bed59b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4423,10 +4423,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K191" sqref="K191"/>
+      <selection pane="bottomRight" activeCell="H197" sqref="H197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4738,7 +4738,7 @@
         <v>318</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="M10" s="34"/>
       <c r="N10" s="34"/>
@@ -4781,7 +4781,7 @@
         <v>318</v>
       </c>
       <c r="L11" s="34" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
@@ -4824,7 +4824,7 @@
         <v>318</v>
       </c>
       <c r="L12" s="34" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -4867,7 +4867,7 @@
         <v>318</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
@@ -4910,7 +4910,7 @@
         <v>318</v>
       </c>
       <c r="L14" s="34" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
@@ -5538,13 +5538,13 @@
         <v>45695</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="H31" s="33" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="I31" s="33" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="J31" s="34" t="s">
         <v>87</v>
@@ -5558,7 +5558,7 @@
         <v>87</v>
       </c>
       <c r="O31" s="34" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="P31" s="34" t="s">
         <v>87</v>
@@ -5570,7 +5570,7 @@
         <v>87</v>
       </c>
       <c r="S31" s="34" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="T31" s="34"/>
       <c r="U31" s="35"/>
@@ -5858,13 +5858,13 @@
         <v>45695</v>
       </c>
       <c r="G39" s="33" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="H39" s="33" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="I39" s="33" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="J39" s="34" t="s">
         <v>87</v>
@@ -5878,7 +5878,7 @@
         <v>87</v>
       </c>
       <c r="O39" s="34" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="P39" s="34" t="s">
         <v>87</v>
@@ -5890,7 +5890,7 @@
         <v>87</v>
       </c>
       <c r="S39" s="34" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="T39" s="34"/>
       <c r="U39" s="35"/>
@@ -6192,7 +6192,7 @@
         <v>87</v>
       </c>
       <c r="O47" s="34" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="P47" s="34" t="s">
         <v>87</v>
@@ -6204,7 +6204,7 @@
         <v>87</v>
       </c>
       <c r="S47" s="34" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="T47" s="34"/>
       <c r="U47" s="35" t="s">
@@ -6515,7 +6515,7 @@
         <v>318</v>
       </c>
       <c r="L55" s="34" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="M55" s="34"/>
       <c r="N55" s="34"/>
@@ -6558,7 +6558,7 @@
         <v>318</v>
       </c>
       <c r="L56" s="34" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="M56" s="34"/>
       <c r="N56" s="34"/>
@@ -6601,7 +6601,7 @@
         <v>318</v>
       </c>
       <c r="L57" s="34" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="M57" s="34"/>
       <c r="N57" s="34"/>
@@ -6644,7 +6644,7 @@
         <v>318</v>
       </c>
       <c r="L58" s="34" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="M58" s="34"/>
       <c r="N58" s="34"/>
@@ -6687,7 +6687,7 @@
         <v>318</v>
       </c>
       <c r="L59" s="34" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="M59" s="34"/>
       <c r="N59" s="34"/>
@@ -6771,7 +6771,7 @@
         <v>318</v>
       </c>
       <c r="L61" s="34" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="M61" s="34"/>
       <c r="N61" s="34"/>
@@ -6814,7 +6814,7 @@
         <v>318</v>
       </c>
       <c r="L62" s="34" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="M62" s="34"/>
       <c r="N62" s="34"/>
@@ -6850,13 +6850,13 @@
         <v>45698</v>
       </c>
       <c r="G63" s="33" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="H63" s="33" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="I63" s="33" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="J63" s="34" t="s">
         <v>87</v>
@@ -6870,7 +6870,7 @@
         <v>87</v>
       </c>
       <c r="O63" s="34" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="P63" s="34" t="s">
         <v>87</v>
@@ -6882,7 +6882,7 @@
         <v>87</v>
       </c>
       <c r="S63" s="34" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="T63" s="34"/>
       <c r="U63" s="35"/>
@@ -6918,7 +6918,7 @@
         <v>318</v>
       </c>
       <c r="L64" s="34" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="M64" s="34"/>
       <c r="N64" s="34"/>
@@ -6961,7 +6961,7 @@
         <v>318</v>
       </c>
       <c r="L65" s="34" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="M65" s="34"/>
       <c r="N65" s="34"/>
@@ -11582,16 +11582,16 @@
         <v>476</v>
       </c>
       <c r="F190" s="32">
-        <v>45695</v>
+        <v>45708</v>
       </c>
       <c r="G190" s="33" t="s">
-        <v>493</v>
+        <v>522</v>
       </c>
       <c r="H190" s="33" t="s">
-        <v>494</v>
+        <v>523</v>
       </c>
       <c r="I190" s="33" t="s">
-        <v>495</v>
+        <v>524</v>
       </c>
       <c r="J190" s="34" t="s">
         <v>87</v>
@@ -11632,13 +11632,13 @@
         <v>45695</v>
       </c>
       <c r="G191" s="33" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="H191" s="33" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="I191" s="33" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="J191" s="34" t="s">
         <v>87</v>
@@ -11861,16 +11861,16 @@
         <v>483</v>
       </c>
       <c r="F197" s="44">
-        <v>45695</v>
+        <v>45708</v>
       </c>
       <c r="G197" s="45" t="s">
-        <v>497</v>
+        <v>526</v>
       </c>
       <c r="H197" s="45" t="s">
-        <v>496</v>
+        <v>525</v>
       </c>
       <c r="I197" s="45" t="s">
-        <v>498</v>
+        <v>527</v>
       </c>
       <c r="J197" s="46" t="s">
         <v>87</v>
@@ -19103,15 +19103,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19373,27 +19370,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19418,9 +19409,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TESI SPA - EMOWEB - Accreditamento - II Correzione Test Case
TESI SPA - EMOWEB - Accreditamento - Seconda Correzione Test Case (191 e 376)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250220\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250303\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FEA541-0885-4900-B9E5-3058F4A381AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF883E-40A4-487F-88AF-467A1DD7E959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2013,22 +2013,22 @@
     <t>2.16.840.1.113883.2.9.2.190208.6.11.b7e3599442e9321114b7a048d8b6ca9b583fb36ec4fab58754e98a9ff5f7abb7.99918db4c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2025-02-20T16:16:11.643Z</t>
-  </si>
-  <si>
-    <t>ec0fb70c78870364</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.7efbaea588^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>56e8705b885bb22f</t>
-  </si>
-  <si>
-    <t>2025-02-20T16:22:03.068Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.5f58bed59b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>acf24b83b25230a4</t>
+  </si>
+  <si>
+    <t>2025-03-03T07:06:22.290Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.109369712a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5fbcb3cabf76f238</t>
+  </si>
+  <si>
+    <t>2025-03-03T07:06:41.090Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.222e3ce660^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4423,10 +4423,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H197" sqref="H197"/>
+      <selection pane="bottomRight" activeCell="I197" sqref="I197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4711,7 +4711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>2</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>3</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>4</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>5</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="29">
         <v>179</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="29">
         <v>180</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="29">
         <v>181</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="29">
         <v>182</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="29">
         <v>183</v>
       </c>
@@ -11306,7 +11306,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="29">
         <v>184</v>
       </c>
@@ -11343,7 +11343,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="29">
         <v>185</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="29">
         <v>186</v>
       </c>
@@ -11417,7 +11417,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="29">
         <v>187</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="29">
         <v>188</v>
       </c>
@@ -11491,7 +11491,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="29">
         <v>189</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="29">
         <v>190</v>
       </c>
@@ -11582,13 +11582,13 @@
         <v>476</v>
       </c>
       <c r="F190" s="32">
-        <v>45708</v>
+        <v>45719</v>
       </c>
       <c r="G190" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="H190" s="33" t="s">
         <v>522</v>
-      </c>
-      <c r="H190" s="33" t="s">
-        <v>523</v>
       </c>
       <c r="I190" s="33" t="s">
         <v>524</v>
@@ -11861,7 +11861,7 @@
         <v>483</v>
       </c>
       <c r="F197" s="44">
-        <v>45708</v>
+        <v>45719</v>
       </c>
       <c r="G197" s="45" t="s">
         <v>526</v>
@@ -19103,15 +19103,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19369,6 +19360,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -19382,14 +19382,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19404,6 +19396,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Revert "TESI SPA - EMOWEB - Accreditamento - II Correzione Test Case"
This reverts commit d7bcfaffe8c96f9c7f47f6af2af0daba264eda0a.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250303\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250220\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF883E-40A4-487F-88AF-467A1DD7E959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FEA541-0885-4900-B9E5-3058F4A381AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2013,22 +2013,22 @@
     <t>2.16.840.1.113883.2.9.2.190208.6.11.b7e3599442e9321114b7a048d8b6ca9b583fb36ec4fab58754e98a9ff5f7abb7.99918db4c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>acf24b83b25230a4</t>
-  </si>
-  <si>
-    <t>2025-03-03T07:06:22.290Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.109369712a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5fbcb3cabf76f238</t>
-  </si>
-  <si>
-    <t>2025-03-03T07:06:41.090Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.222e3ce660^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-02-20T16:16:11.643Z</t>
+  </si>
+  <si>
+    <t>ec0fb70c78870364</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.7efbaea588^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>56e8705b885bb22f</t>
+  </si>
+  <si>
+    <t>2025-02-20T16:22:03.068Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.5f58bed59b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4423,10 +4423,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I197" sqref="I197"/>
+      <selection pane="bottomRight" activeCell="H197" sqref="H197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4711,7 +4711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>2</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>3</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>4</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>5</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="29">
         <v>179</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="29">
         <v>180</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="29">
         <v>181</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="29">
         <v>182</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="29">
         <v>183</v>
       </c>
@@ -11306,7 +11306,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="29">
         <v>184</v>
       </c>
@@ -11343,7 +11343,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="29">
         <v>185</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="29">
         <v>186</v>
       </c>
@@ -11417,7 +11417,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="29">
         <v>187</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="29">
         <v>188</v>
       </c>
@@ -11491,7 +11491,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="29">
         <v>189</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="29">
         <v>190</v>
       </c>
@@ -11582,13 +11582,13 @@
         <v>476</v>
       </c>
       <c r="F190" s="32">
-        <v>45719</v>
+        <v>45708</v>
       </c>
       <c r="G190" s="33" t="s">
+        <v>522</v>
+      </c>
+      <c r="H190" s="33" t="s">
         <v>523</v>
-      </c>
-      <c r="H190" s="33" t="s">
-        <v>522</v>
       </c>
       <c r="I190" s="33" t="s">
         <v>524</v>
@@ -11861,7 +11861,7 @@
         <v>483</v>
       </c>
       <c r="F197" s="44">
-        <v>45719</v>
+        <v>45708</v>
       </c>
       <c r="G197" s="45" t="s">
         <v>526</v>
@@ -19103,6 +19103,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19360,15 +19369,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -19382,6 +19382,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19396,14 +19404,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
TESI SPA - EMOWEB - Correzione test case 191 e 376
Secondo caricamento della correzione dei test case 191 e 376
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250220\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250303\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FEA541-0885-4900-B9E5-3058F4A381AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF883E-40A4-487F-88AF-467A1DD7E959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2013,22 +2013,22 @@
     <t>2.16.840.1.113883.2.9.2.190208.6.11.b7e3599442e9321114b7a048d8b6ca9b583fb36ec4fab58754e98a9ff5f7abb7.99918db4c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2025-02-20T16:16:11.643Z</t>
-  </si>
-  <si>
-    <t>ec0fb70c78870364</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.7efbaea588^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>56e8705b885bb22f</t>
-  </si>
-  <si>
-    <t>2025-02-20T16:22:03.068Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.5f58bed59b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>acf24b83b25230a4</t>
+  </si>
+  <si>
+    <t>2025-03-03T07:06:22.290Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.109369712a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5fbcb3cabf76f238</t>
+  </si>
+  <si>
+    <t>2025-03-03T07:06:41.090Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.222e3ce660^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4423,10 +4423,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H197" sqref="H197"/>
+      <selection pane="bottomRight" activeCell="I197" sqref="I197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4711,7 +4711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>2</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>3</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>4</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>5</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="29">
         <v>179</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="29">
         <v>180</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="29">
         <v>181</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="29">
         <v>182</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="29">
         <v>183</v>
       </c>
@@ -11306,7 +11306,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="29">
         <v>184</v>
       </c>
@@ -11343,7 +11343,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="29">
         <v>185</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="29">
         <v>186</v>
       </c>
@@ -11417,7 +11417,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="29">
         <v>187</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="29">
         <v>188</v>
       </c>
@@ -11491,7 +11491,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="29">
         <v>189</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="29">
         <v>190</v>
       </c>
@@ -11582,13 +11582,13 @@
         <v>476</v>
       </c>
       <c r="F190" s="32">
-        <v>45708</v>
+        <v>45719</v>
       </c>
       <c r="G190" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="H190" s="33" t="s">
         <v>522</v>
-      </c>
-      <c r="H190" s="33" t="s">
-        <v>523</v>
       </c>
       <c r="I190" s="33" t="s">
         <v>524</v>
@@ -11861,7 +11861,7 @@
         <v>483</v>
       </c>
       <c r="F197" s="44">
-        <v>45708</v>
+        <v>45719</v>
       </c>
       <c r="G197" s="45" t="s">
         <v>526</v>
@@ -19103,15 +19103,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19369,6 +19360,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -19382,14 +19382,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19404,6 +19396,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
TESI SPA - EMOWEB - Correzione test 191 e 376
TESI SPA - EMOWEB (TRASFUSIONALE) Seconda correzione test case 191 e 376
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/EMOWEB/3.3/EMOWEB_accreditamento-checklist_V8.2.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250220\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\EMOWEB\20250303\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FEA541-0885-4900-B9E5-3058F4A381AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF883E-40A4-487F-88AF-467A1DD7E959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2013,22 +2013,22 @@
     <t>2.16.840.1.113883.2.9.2.190208.6.11.b7e3599442e9321114b7a048d8b6ca9b583fb36ec4fab58754e98a9ff5f7abb7.99918db4c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2025-02-20T16:16:11.643Z</t>
-  </si>
-  <si>
-    <t>ec0fb70c78870364</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.7efbaea588^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>56e8705b885bb22f</t>
-  </si>
-  <si>
-    <t>2025-02-20T16:22:03.068Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.5f58bed59b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>acf24b83b25230a4</t>
+  </si>
+  <si>
+    <t>2025-03-03T07:06:22.290Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.bb77a5b3c29256af01e8e576c7c45994042aa641c162eeb6efc0ea808f865b5e.109369712a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5fbcb3cabf76f238</t>
+  </si>
+  <si>
+    <t>2025-03-03T07:06:41.090Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190208.6.11.12fc6a3e05046a7088edd259108b636aa4d76fa4a7d61c018ea4283a40de3983.222e3ce660^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4423,10 +4423,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H197" sqref="H197"/>
+      <selection pane="bottomRight" activeCell="I197" sqref="I197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4711,7 +4711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>2</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>3</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>4</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>5</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="29">
         <v>179</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="29">
         <v>180</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="29">
         <v>181</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="29">
         <v>182</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="29">
         <v>183</v>
       </c>
@@ -11306,7 +11306,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="29">
         <v>184</v>
       </c>
@@ -11343,7 +11343,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="29">
         <v>185</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="29">
         <v>186</v>
       </c>
@@ -11417,7 +11417,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="29">
         <v>187</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="29">
         <v>188</v>
       </c>
@@ -11491,7 +11491,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="29">
         <v>189</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="29">
         <v>190</v>
       </c>
@@ -11582,13 +11582,13 @@
         <v>476</v>
       </c>
       <c r="F190" s="32">
-        <v>45708</v>
+        <v>45719</v>
       </c>
       <c r="G190" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="H190" s="33" t="s">
         <v>522</v>
-      </c>
-      <c r="H190" s="33" t="s">
-        <v>523</v>
       </c>
       <c r="I190" s="33" t="s">
         <v>524</v>
@@ -11861,7 +11861,7 @@
         <v>483</v>
       </c>
       <c r="F197" s="44">
-        <v>45708</v>
+        <v>45719</v>
       </c>
       <c r="G197" s="45" t="s">
         <v>526</v>
@@ -19103,15 +19103,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19369,6 +19360,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -19382,14 +19382,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19404,6 +19396,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>